<commit_message>
4-10 redux-saga 구조 잡기 완료
</commit_message>
<xml_diff>
--- a/React강좌.xlsx
+++ b/React강좌.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Seok\Desktop\개발\Graduate\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB1D3E00-33A7-46B6-8931-ED4D5274224F}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8094E8F0-9A16-4C3E-B843-DA6126292AF3}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="32340" yWindow="2580" windowWidth="2400" windowHeight="585" activeTab="3" xr2:uid="{8D8F7A3E-3A4C-48EA-AE50-53AF22253C3F}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{8D8F7A3E-3A4C-48EA-AE50-53AF22253C3F}"/>
   </bookViews>
   <sheets>
     <sheet name="REACT" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="57">
   <si>
     <t>React 강좌</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -236,21 +236,11 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>call은 함수 동기적 호출
-fork는 함수 비동기적 호출
-put은 액션 dispatch</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>미들웨어 만드는 방법 : (currying 기법 - 인자 하나를 받아 다른 함수를 리턴)
 const middleware = (store) =&gt; (next) =&gt; (action) =&gt;{
  console.log(action); // 다른 작업들은 여기에
  next(action);
 };</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>제너레이터는 함수 실행을 준간에 멈출 수 있고 기존 컴포넌트에 props같은 것을 추가할 때 쓴다.</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -292,8 +282,54 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>call은 함수 동기적 호출 : 요청 보내고 응답을 다받을 때까지 기다림
+fork는 함수 비동기적 호출 : 요청 보내고 응답받지 않아도 다음 실행
+put은 액션 dispatch</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>race, cancel, select, throttle, debounce 이펙트 어떤용도 인지 확인하기
+race : 제일 먼저 도달에 성공한 함수만을 실행 시킨다.
+yield race({
+        waitting: delay(200),
+        stoped: take(getType(Actions.stopMonitoring))
+      });
+위의 코드에서 액션 타입이 stopMonitoring으로 바뀌지 않는 한 계속 waitting이 이긴다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>select : 사가의 제너레이터 안에서 스토어의 상태를 가지고 올 때, 스토어 전체를 리턴한다.
+Const { monitoring, monitoringDuration } = yield select();</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>getType : 액션의 타입 값을 뽑아내는 함수
+import { getType } from "typesafe-actions";
+import * as Actions from "../actions";
+getType(Actions.startMonitoring);</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>cancel : 포크되었던 서브 프로세스를 취소한다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>제너레이터는 함수 실행을 중간에 멈출 수 있고 기존 컴포넌트에 props같은 것을 추가할 때 쓴다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>takeLatest : 이전 요청이 끝나지 않은게 있다면 이전 요청을 취소한다.
-동시에 여러 번 실행하면 마지막것만 받을 수 있음 -&gt; 로그인 버튼을 막누르면 서버로 여러 개 가는것을 제어헤줄 수 있음</t>
+동시에 여러 번 실행하면 마지막것만 받을 수 있음 -&gt; 로그인 버튼을 막누르면 서버로 여러 개 가는것을 제어헤줄 수 있음
+takeEvery와 takeLatest중 어떤것을 선택할까 고민될때 생각할때 예제
+버튼을 클릭할때마다 카운트가 1씩 증가해야한다. Every, 여러번중 한번만 선택되게한다 Latest</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>비동기일경우 다움과 같은 형식을 쓰면 좋음 (서버쪽에 갓다 와야하는 구나 -&gt; 리덕스 사가를 써야 겠구나)
+A_REQUEST
+A_SUCCESS
+A_FAILURE
+동기는 하나로 떨어지므로 리덕스만으로 처리 가능</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -900,8 +936,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8819C134-92EB-4092-95A4-2C8F254EB41D}">
   <dimension ref="A1:C15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -994,8 +1030,10 @@
         <v>34</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A15" s="1"/>
+    <row r="15" spans="1:3" ht="99" x14ac:dyDescent="0.3">
+      <c r="A15" s="1" t="s">
+        <v>56</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
@@ -1006,10 +1044,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2B2169FF-6B20-40D7-8BD4-C1BE4486CE85}">
-  <dimension ref="A1:C17"/>
+  <dimension ref="A1:C21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1061,12 +1099,12 @@
     </row>
     <row r="8" spans="1:3" ht="49.5" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
-        <v>42</v>
+        <v>49</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="81" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B9" t="s">
         <v>29</v>
@@ -1074,42 +1112,62 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
-        <v>44</v>
+        <v>54</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="280.5" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="30.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" ht="66" x14ac:dyDescent="0.3">
+      <c r="A17" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" ht="115.5" x14ac:dyDescent="0.3">
+      <c r="A18" s="1" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="17" spans="1:1" ht="33" x14ac:dyDescent="0.3">
-      <c r="A17" s="1" t="s">
+    <row r="19" spans="1:1" ht="33" x14ac:dyDescent="0.3">
+      <c r="A19" s="1" t="s">
         <v>51</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" ht="82.5" x14ac:dyDescent="0.3">
+      <c r="A20" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A21" s="1" t="s">
+        <v>53</v>
       </c>
     </row>
   </sheetData>

</xml_diff>